<commit_message>
Fixes according to TODO list
</commit_message>
<xml_diff>
--- a/inventory/reports/scheme/umk.xlsx
+++ b/inventory/reports/scheme/umk.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Район</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Заказы (экз.)</t>
+  </si>
+  <si>
+    <t>Инвентаризация (экз.)</t>
+  </si>
+  <si>
+    <t>Потребность (экз.)</t>
   </si>
 </sst>
 </file>
@@ -150,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -162,32 +171,35 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,34 +507,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="H2" sqref="H2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="33" style="11" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="23.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="33" style="9" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="11" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15" style="14" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -544,184 +559,193 @@
       <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G2"/>
+  <autoFilter ref="A2:J2"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>